<commit_message>
HW REV 1.3 : added Cu requirement 2oz/ft^2, checked insolation and track width
delta T = 45°C with I=15A with 2 oz/ft^2
</commit_message>
<xml_diff>
--- a/hardware/rev 1.3/BOM_FAB-O-MATIC_PCB REV1.3_2024-08-18.xlsx
+++ b/hardware/rev 1.3/BOM_FAB-O-MATIC_PCB REV1.3_2024-08-18.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="190">
   <si>
     <t>No.</t>
   </si>
@@ -235,7 +235,7 @@
     <t>Jumper</t>
   </si>
   <si>
-    <t>J1</t>
+    <t>J1,J2,J3</t>
   </si>
   <si>
     <t>JUMPER</t>
@@ -376,211 +376,196 @@
     <t>19</t>
   </si>
   <si>
-    <t>22Ω</t>
-  </si>
-  <si>
-    <t>R4,R5</t>
+    <t>100kΩ</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>0805W8F1003T5E</t>
+  </si>
+  <si>
+    <t>C149504</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>R7,R13,R14,R15</t>
   </si>
   <si>
     <t>R0603</t>
   </si>
   <si>
-    <t>0603WAF220JT5E</t>
-  </si>
-  <si>
-    <t>C23345</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>100kΩ</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>0805W8F1003T5E</t>
-  </si>
-  <si>
-    <t>C149504</t>
+    <t>0603WAF1003T5E</t>
+  </si>
+  <si>
+    <t>C25803</t>
   </si>
   <si>
     <t>21</t>
   </si>
   <si>
-    <t>R7,R13,R14,R15</t>
-  </si>
-  <si>
-    <t>0603WAF1003T5E</t>
-  </si>
-  <si>
-    <t>C25803</t>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>RES-ADJ-TH_3362P</t>
+  </si>
+  <si>
+    <t>3362P-1-103</t>
+  </si>
+  <si>
+    <t>BOCHEN(博晨)</t>
+  </si>
+  <si>
+    <t>C118956</t>
   </si>
   <si>
     <t>22</t>
   </si>
   <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>RES-ADJ-TH_3362P</t>
-  </si>
-  <si>
-    <t>3362P-1-103</t>
-  </si>
-  <si>
-    <t>BOCHEN(博晨)</t>
-  </si>
-  <si>
-    <t>C118956</t>
+    <t>127kΩ</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>RC0603FR-07127KL</t>
+  </si>
+  <si>
+    <t>C245905</t>
   </si>
   <si>
     <t>23</t>
   </si>
   <si>
-    <t>127kΩ</t>
-  </si>
-  <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>RC0603FR-07127KL</t>
-  </si>
-  <si>
-    <t>C245905</t>
+    <t>5.1kΩ</t>
+  </si>
+  <si>
+    <t>R10,R12</t>
+  </si>
+  <si>
+    <t>0603WAF5101T5E</t>
+  </si>
+  <si>
+    <t>C23186</t>
   </si>
   <si>
     <t>24</t>
   </si>
   <si>
-    <t>5.1kΩ</t>
-  </si>
-  <si>
-    <t>R10,R12</t>
-  </si>
-  <si>
-    <t>0603WAF5101T5E</t>
-  </si>
-  <si>
-    <t>C23186</t>
+    <t>24kΩ</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>0603WAF2402T5E</t>
+  </si>
+  <si>
+    <t>C23352</t>
   </si>
   <si>
     <t>25</t>
   </si>
   <si>
-    <t>24kΩ</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>0603WAF2402T5E</t>
-  </si>
-  <si>
-    <t>C23352</t>
+    <t>ESP32-S3-WROOM-1-N4R8</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>wirelm-smd_esp32-s3-wroom-1</t>
+  </si>
+  <si>
+    <t>ESPRESSIF(乐鑫)</t>
+  </si>
+  <si>
+    <t>C2913200</t>
   </si>
   <si>
     <t>26</t>
   </si>
   <si>
-    <t>ESP32-S3-WROOM-1-N4R8</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>wirelm-smd_esp32-s3-wroom-1</t>
-  </si>
-  <si>
-    <t>ESPRESSIF(乐鑫)</t>
-  </si>
-  <si>
-    <t>C2913200</t>
+    <t>LD1117S33TR</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>SOT-223_L6.5-W3.5-P2.30-LS7.0-BR</t>
+  </si>
+  <si>
+    <t>ST(意法半导体)</t>
+  </si>
+  <si>
+    <t>C86781</t>
   </si>
   <si>
     <t>27</t>
   </si>
   <si>
-    <t>LD1117S33TR</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>SOT-223_L6.5-W3.5-P2.30-LS7.0-BR</t>
-  </si>
-  <si>
-    <t>ST(意法半导体)</t>
-  </si>
-  <si>
-    <t>C86781</t>
+    <t>TP6841S6-A</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>C2844924</t>
   </si>
   <si>
     <t>28</t>
   </si>
   <si>
-    <t>TP6841S6-A</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>C2844924</t>
+    <t>LCD-1602</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>footprint_8a57</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
   <si>
     <t>29</t>
   </si>
   <si>
-    <t>LCD-1602</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>footprint_8a57</t>
-  </si>
-  <si>
-    <t>?</t>
+    <t>MMBT3906</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>SOT-23-3_L2.9-W1.3-P1.90-LS2.4-BR</t>
+  </si>
+  <si>
+    <t>宏迦橙</t>
+  </si>
+  <si>
+    <t>C7420354</t>
   </si>
   <si>
     <t>30</t>
   </si>
   <si>
-    <t>MMBT3906</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>SOT-23-3_L2.9-W1.3-P1.90-LS2.4-BR</t>
-  </si>
-  <si>
-    <t>宏迦橙</t>
-  </si>
-  <si>
-    <t>C7420354</t>
+    <t>DB103-5.0-4P-GN-S</t>
+  </si>
+  <si>
+    <t>U8,U9</t>
+  </si>
+  <si>
+    <t>CONN-TH_4P-P5.00_DB103-5.0-4P-GN-S</t>
+  </si>
+  <si>
+    <t>DORABO(地博电气)</t>
+  </si>
+  <si>
+    <t>C430585</t>
   </si>
   <si>
     <t>31</t>
-  </si>
-  <si>
-    <t>DB103-5.0-4P-GN-S</t>
-  </si>
-  <si>
-    <t>U8,U9</t>
-  </si>
-  <si>
-    <t>CONN-TH_4P-P5.00_DB103-5.0-4P-GN-S</t>
-  </si>
-  <si>
-    <t>DORABO(地博电气)</t>
-  </si>
-  <si>
-    <t>C430585</t>
-  </si>
-  <si>
-    <t>32</t>
   </si>
   <si>
     <t>U262-161N-4BVC11</t>
@@ -972,7 +957,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -1338,7 +1323,7 @@
         <v>72</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
         <v>73</v>
@@ -1594,7 +1579,7 @@
         <v>120</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
         <v>121</v>
@@ -1603,19 +1588,19 @@
         <v>122</v>
       </c>
       <c r="E20" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="F20" t="s">
         <v>121</v>
       </c>
       <c r="G20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H20" t="s">
         <v>113</v>
       </c>
       <c r="I20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J20" t="s">
         <v>17</v>
@@ -1623,31 +1608,31 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" t="s">
         <v>126</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>127</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F21" t="s">
+        <v>121</v>
+      </c>
+      <c r="G21" t="s">
         <v>128</v>
-      </c>
-      <c r="E21" t="s">
-        <v>111</v>
-      </c>
-      <c r="F21" t="s">
-        <v>127</v>
-      </c>
-      <c r="G21" t="s">
-        <v>129</v>
       </c>
       <c r="H21" t="s">
         <v>113</v>
       </c>
       <c r="I21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J21" t="s">
         <v>17</v>
@@ -1655,31 +1640,31 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" t="s">
         <v>131</v>
       </c>
-      <c r="B22">
-        <v>4</v>
-      </c>
-      <c r="C22" t="s">
-        <v>127</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>132</v>
       </c>
-      <c r="E22" t="s">
-        <v>123</v>
-      </c>
       <c r="F22" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="G22" t="s">
         <v>133</v>
       </c>
       <c r="H22" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="I22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J22" t="s">
         <v>17</v>
@@ -1687,28 +1672,28 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="D23" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E23" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" t="s">
         <v>137</v>
       </c>
-      <c r="F23" t="s">
-        <v>109</v>
-      </c>
       <c r="G23" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H23" t="s">
-        <v>139</v>
+        <v>45</v>
       </c>
       <c r="I23" t="s">
         <v>140</v>
@@ -1722,7 +1707,7 @@
         <v>141</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
         <v>142</v>
@@ -1731,7 +1716,7 @@
         <v>143</v>
       </c>
       <c r="E24" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F24" t="s">
         <v>142</v>
@@ -1740,7 +1725,7 @@
         <v>144</v>
       </c>
       <c r="H24" t="s">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="I24" t="s">
         <v>145</v>
@@ -1754,7 +1739,7 @@
         <v>146</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
         <v>147</v>
@@ -1763,7 +1748,7 @@
         <v>148</v>
       </c>
       <c r="E25" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F25" t="s">
         <v>147</v>
@@ -1795,19 +1780,19 @@
         <v>153</v>
       </c>
       <c r="E26" t="s">
-        <v>123</v>
+        <v>154</v>
       </c>
       <c r="F26" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" t="s">
         <v>152</v>
       </c>
-      <c r="G26" t="s">
-        <v>154</v>
-      </c>
       <c r="H26" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="I26" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J26" t="s">
         <v>17</v>
@@ -1815,31 +1800,31 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E27" t="s">
+        <v>160</v>
+      </c>
+      <c r="F27" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" t="s">
         <v>158</v>
       </c>
-      <c r="E27" t="s">
-        <v>159</v>
-      </c>
-      <c r="F27" t="s">
-        <v>58</v>
-      </c>
-      <c r="G27" t="s">
-        <v>157</v>
-      </c>
       <c r="H27" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I27" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J27" t="s">
         <v>17</v>
@@ -1847,31 +1832,31 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D28" t="s">
+        <v>165</v>
+      </c>
+      <c r="E28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" t="s">
         <v>164</v>
       </c>
-      <c r="E28" t="s">
-        <v>165</v>
-      </c>
-      <c r="F28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G28" t="s">
-        <v>163</v>
-      </c>
       <c r="H28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I28" t="s">
         <v>166</v>
-      </c>
-      <c r="I28" t="s">
-        <v>167</v>
       </c>
       <c r="J28" t="s">
         <v>17</v>
@@ -1879,34 +1864,34 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
+        <v>168</v>
+      </c>
+      <c r="D29" t="s">
         <v>169</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>170</v>
       </c>
-      <c r="E29" t="s">
-        <v>64</v>
-      </c>
       <c r="F29" t="s">
         <v>58</v>
       </c>
       <c r="G29" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H29" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="I29" t="s">
-        <v>171</v>
+        <v>58</v>
       </c>
       <c r="J29" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1929,45 +1914,45 @@
         <v>58</v>
       </c>
       <c r="G30" t="s">
+        <v>173</v>
+      </c>
+      <c r="H30" t="s">
         <v>176</v>
       </c>
-      <c r="H30" t="s">
-        <v>58</v>
-      </c>
       <c r="I30" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="J30" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D31" t="s">
+        <v>180</v>
+      </c>
+      <c r="E31" t="s">
+        <v>181</v>
+      </c>
+      <c r="F31" t="s">
+        <v>58</v>
+      </c>
+      <c r="G31" t="s">
         <v>179</v>
       </c>
-      <c r="E31" t="s">
-        <v>180</v>
-      </c>
-      <c r="F31" t="s">
-        <v>58</v>
-      </c>
-      <c r="G31" t="s">
-        <v>178</v>
-      </c>
       <c r="H31" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I31" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="J31" t="s">
         <v>17</v>
@@ -1975,70 +1960,38 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D32" t="s">
+        <v>186</v>
+      </c>
+      <c r="E32" t="s">
+        <v>187</v>
+      </c>
+      <c r="F32" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" t="s">
         <v>185</v>
       </c>
-      <c r="E32" t="s">
-        <v>186</v>
-      </c>
-      <c r="F32" t="s">
-        <v>58</v>
-      </c>
-      <c r="G32" t="s">
-        <v>184</v>
-      </c>
       <c r="H32" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I32" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="J32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>189</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
-        <v>190</v>
-      </c>
-      <c r="D33" t="s">
-        <v>191</v>
-      </c>
-      <c r="E33" t="s">
-        <v>192</v>
-      </c>
-      <c r="F33" t="s">
-        <v>58</v>
-      </c>
-      <c r="G33" t="s">
-        <v>190</v>
-      </c>
-      <c r="H33" t="s">
-        <v>193</v>
-      </c>
-      <c r="I33" t="s">
-        <v>194</v>
-      </c>
-      <c r="J33" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>